<commit_message>
Finalizando mesa da aula10 de POO
</commit_message>
<xml_diff>
--- a/Turma 6/Testing l/Módulo 1 [Fundamentos de Teste e Gestão de Defeitos]/A5A [Níveis e Tipos de Testes]/Caso de Uso  Comida Ya ! [Mesa].xlsx
+++ b/Turma 6/Testing l/Módulo 1 [Fundamentos de Teste e Gestão de Defeitos]/A5A [Níveis e Tipos de Testes]/Caso de Uso  Comida Ya ! [Mesa].xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Desktop\CTD\Turma 6\Testing l\Módulo 1 [Fundamentos de Teste e Gestão de Defeitos]\A5A [Níveis e Tipos de Testes]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6F6051-18C9-4440-A470-284981F4A0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0AE3A0-CCFA-4937-A148-A6C2B1ECC8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{4F8A38D9-B9C1-42D6-AEB2-396C93C0EC4D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4F8A38D9-B9C1-42D6-AEB2-396C93C0EC4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Nome do Tester:</t>
   </si>
@@ -85,24 +85,12 @@
     <t>EVIDÊNCIAS</t>
   </si>
   <si>
-    <t>LOGIN</t>
-  </si>
-  <si>
     <t>Douglas Nascimento</t>
   </si>
   <si>
-    <t>Você deve conseguir adicionar produtos ao carrinho de compras.</t>
-  </si>
-  <si>
     <t>A soma dos preços dos produtos no carrinho de compras deve ser sempre positiva.</t>
   </si>
   <si>
-    <t>O usuário pode fazer login com um nome de usuário e senha.</t>
-  </si>
-  <si>
-    <t>PRODUCTOS</t>
-  </si>
-  <si>
     <t>CARRITO</t>
   </si>
   <si>
@@ -113,6 +101,30 @@
   </si>
   <si>
     <t>LOGOUT</t>
+  </si>
+  <si>
+    <t>Usuário ser redirecionado para a Home</t>
+  </si>
+  <si>
+    <t>Ter apenas alimentos na Home</t>
+  </si>
+  <si>
+    <t>LOGIN (Positivo)</t>
+  </si>
+  <si>
+    <t>Cadastrar  um produto diferente de um alimento</t>
+  </si>
+  <si>
+    <t>HOME (Negativo)</t>
+  </si>
+  <si>
+    <t>Usuário entrar no Comida Ya! Com credenciais válidas</t>
+  </si>
+  <si>
+    <t>Foi possível cadastrar produtos diferentes de alimentos.</t>
+  </si>
+  <si>
+    <t>Usuário foi redirecionado para a página Home.</t>
   </si>
 </sst>
 </file>
@@ -410,10 +422,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -733,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7072082B-18AF-40DB-A58A-DF7A3E5CFFC7}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +755,7 @@
     <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -753,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -842,56 +854,66 @@
         <v>1</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:26" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:26" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
-        <v>4</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>22</v>
+        <v>3</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>18</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:26" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
-        <v>5</v>
-      </c>
-      <c r="B12" s="20"/>
+        <v>4</v>
+      </c>
+      <c r="B12" s="21"/>
       <c r="C12" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:26" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5"/>
     </row>

</xml_diff>